<commit_message>
New simplified config system (working, but needs extensive testing)
PREV VERSION WORKED
</commit_message>
<xml_diff>
--- a/reference/dictionaries/EE.xlsx
+++ b/reference/dictionaries/EE.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.humphreys\Documents\Development\EHR-BSI-TryingHarmonisedExcel\reference\dictionaries\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8366DE5F-77FF-4F70-B585-412BDCA2B16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
-    <sheet name="Lookups" sheetId="2" r:id="rId2"/>
+    <sheet name="Dictionary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Lookups" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Config" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="394">
   <si>
     <t>raw_column_name</t>
   </si>
@@ -218,7 +212,7 @@
     <t>UNK</t>
   </si>
   <si>
-    <t/>
+    <t>NA</t>
   </si>
   <si>
     <t>URO</t>
@@ -1012,13 +1006,209 @@
   </si>
   <si>
     <t>HospitalType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config_key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%d/%m/%Y %H:%M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DateOfSpecCollection,DateOfHospitalAdmission,DateOfHospitalDischarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">record_id_bsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{HospitalId}-{year}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">record_id_patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{PatientId}-{admit_datetime}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">record_id_isolate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{IsolateId}_{MicroorganismCode}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibiotic_format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibiotic_test_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivityTest_noncdm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibiotic_result_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivityResult_noncdm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibiotic_value_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivityValue_noncdm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibiotic_unit_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivityUnit_noncdm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibiotic_translation_chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST2ENG,ENG2HAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_type_grad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grad$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_type_mic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MIK$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_type_zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disk$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminology_clinical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICD-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminology_clinical_spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminology_microbiological</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNOMED-CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminology_microbiological_spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">terminology_hospitalisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MecRes,ResRecode,Ab_EST2ENG,Ab_ENG2HAI,HospType,HospGeog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospType_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HospitalId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospType_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estonia_hosptype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospType_to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hosptype_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospType_output_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HospitalType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospGeog_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospGeog_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospGeog_to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuts3_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lookup_mapping_HospGeog_output_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_ehrbsi_ESurvBSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_ehrbsi_HospitalSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_ehrbsi_ProportionPopulationCovered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1344,19 +1534,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -1372,7 +1562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" t="s">
         <v>298</v>
       </c>
@@ -1380,7 +1570,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -1388,7 +1578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -1396,7 +1586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -1404,7 +1594,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" t="s">
         <v>304</v>
       </c>
@@ -1412,7 +1602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" t="s">
         <v>305</v>
       </c>
@@ -1420,7 +1610,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" t="s">
         <v>307</v>
       </c>
@@ -1428,7 +1618,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="A10" t="s">
         <v>309</v>
       </c>
@@ -1436,7 +1626,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="A11" t="s">
         <v>311</v>
       </c>
@@ -1444,7 +1634,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="A12" t="s">
         <v>313</v>
       </c>
@@ -1452,7 +1642,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="A13" t="s">
         <v>315</v>
       </c>
@@ -1460,7 +1650,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="A14" t="s">
         <v>317</v>
       </c>
@@ -1468,7 +1658,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="A15" t="s">
         <v>319</v>
       </c>
@@ -1476,7 +1666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16">
       <c r="A16" t="s">
         <v>320</v>
       </c>
@@ -1484,7 +1674,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17">
       <c r="A17" t="s">
         <v>322</v>
       </c>
@@ -1492,7 +1682,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18">
       <c r="A18" t="s">
         <v>324</v>
       </c>
@@ -1500,7 +1690,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19">
       <c r="A19" t="s">
         <v>326</v>
       </c>
@@ -1508,7 +1698,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20">
       <c r="A20" t="s">
         <v>328</v>
       </c>
@@ -1523,14 +1713,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C260"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1541,7 +1731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +1742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1563,7 +1753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1574,7 +1764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1585,7 +1775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1596,7 +1786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1607,7 +1797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1618,7 +1808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1629,7 +1819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1640,7 +1830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1651,7 +1841,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1662,7 +1852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1673,7 +1863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1684,7 +1874,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1695,7 +1885,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1706,7 +1896,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1717,7 +1907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1728,7 +1918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1739,7 +1929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1750,7 +1940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1761,7 +1951,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1772,7 +1962,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1783,7 +1973,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1794,7 +1984,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1805,7 +1995,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1816,7 +2006,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1827,7 +2017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1838,7 +2028,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1849,7 +2039,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1860,7 +2050,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1871,7 +2061,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1882,7 +2072,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -1893,7 +2083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -1904,7 +2094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1915,7 +2105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1926,7 +2116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -1937,7 +2127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -1948,7 +2138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -1959,7 +2149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -1970,7 +2160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -1981,7 +2171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -1992,7 +2182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -2003,7 +2193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -2014,7 +2204,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -2025,7 +2215,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -2036,7 +2226,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -2047,7 +2237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -2058,7 +2248,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -2069,7 +2259,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -2080,7 +2270,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -2091,7 +2281,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -2102,7 +2292,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -2113,7 +2303,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -2124,7 +2314,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -2135,7 +2325,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -2146,7 +2336,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57">
       <c r="A57" t="s">
         <v>83</v>
       </c>
@@ -2157,7 +2347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -2168,7 +2358,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -2179,7 +2369,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -2190,7 +2380,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -2201,7 +2391,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -2212,7 +2402,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -2223,7 +2413,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -2234,7 +2424,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -2245,7 +2435,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -2256,7 +2446,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -2267,7 +2457,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -2278,7 +2468,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -2289,7 +2479,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -2300,7 +2490,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71">
       <c r="A71" t="s">
         <v>90</v>
       </c>
@@ -2311,7 +2501,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -2322,7 +2512,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73">
       <c r="A73" t="s">
         <v>90</v>
       </c>
@@ -2333,7 +2523,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -2344,7 +2534,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -2355,7 +2545,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -2366,7 +2556,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77">
       <c r="A77" t="s">
         <v>90</v>
       </c>
@@ -2377,7 +2567,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -2388,7 +2578,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -2399,7 +2589,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -2410,7 +2600,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -2421,7 +2611,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2432,7 +2622,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -2443,7 +2633,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2454,7 +2644,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -2465,7 +2655,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -2476,7 +2666,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2487,7 +2677,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -2498,7 +2688,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -2509,7 +2699,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2520,7 +2710,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2531,7 +2721,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2542,7 +2732,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -2553,7 +2743,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -2564,7 +2754,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95">
       <c r="A95" t="s">
         <v>90</v>
       </c>
@@ -2575,7 +2765,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96">
       <c r="A96" t="s">
         <v>90</v>
       </c>
@@ -2586,7 +2776,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -2597,7 +2787,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98">
       <c r="A98" t="s">
         <v>90</v>
       </c>
@@ -2608,7 +2798,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -2619,7 +2809,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100">
       <c r="A100" t="s">
         <v>90</v>
       </c>
@@ -2630,7 +2820,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101">
       <c r="A101" t="s">
         <v>90</v>
       </c>
@@ -2641,7 +2831,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -2652,7 +2842,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103">
       <c r="A103" t="s">
         <v>90</v>
       </c>
@@ -2663,7 +2853,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104">
       <c r="A104" t="s">
         <v>90</v>
       </c>
@@ -2674,7 +2864,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105">
       <c r="A105" t="s">
         <v>90</v>
       </c>
@@ -2685,7 +2875,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106">
       <c r="A106" t="s">
         <v>90</v>
       </c>
@@ -2696,7 +2886,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107">
       <c r="A107" t="s">
         <v>90</v>
       </c>
@@ -2707,7 +2897,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108">
       <c r="A108" t="s">
         <v>90</v>
       </c>
@@ -2718,7 +2908,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109">
       <c r="A109" t="s">
         <v>90</v>
       </c>
@@ -2729,7 +2919,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110">
       <c r="A110" t="s">
         <v>90</v>
       </c>
@@ -2740,7 +2930,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111">
       <c r="A111" t="s">
         <v>90</v>
       </c>
@@ -2751,7 +2941,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112">
       <c r="A112" t="s">
         <v>90</v>
       </c>
@@ -2762,7 +2952,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113">
       <c r="A113" t="s">
         <v>90</v>
       </c>
@@ -2773,7 +2963,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114">
       <c r="A114" t="s">
         <v>90</v>
       </c>
@@ -2784,7 +2974,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115">
       <c r="A115" t="s">
         <v>90</v>
       </c>
@@ -2795,7 +2985,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116">
       <c r="A116" t="s">
         <v>90</v>
       </c>
@@ -2806,7 +2996,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117">
       <c r="A117" t="s">
         <v>90</v>
       </c>
@@ -2817,7 +3007,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118">
       <c r="A118" t="s">
         <v>90</v>
       </c>
@@ -2828,7 +3018,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119">
       <c r="A119" t="s">
         <v>90</v>
       </c>
@@ -2839,7 +3029,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120">
       <c r="A120" t="s">
         <v>90</v>
       </c>
@@ -2850,7 +3040,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121">
       <c r="A121" t="s">
         <v>90</v>
       </c>
@@ -2861,7 +3051,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122">
       <c r="A122" t="s">
         <v>90</v>
       </c>
@@ -2872,7 +3062,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123">
       <c r="A123" t="s">
         <v>90</v>
       </c>
@@ -2883,7 +3073,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124">
       <c r="A124" t="s">
         <v>90</v>
       </c>
@@ -2894,7 +3084,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125">
       <c r="A125" t="s">
         <v>90</v>
       </c>
@@ -2905,7 +3095,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126">
       <c r="A126" t="s">
         <v>90</v>
       </c>
@@ -2916,7 +3106,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127">
       <c r="A127" t="s">
         <v>90</v>
       </c>
@@ -2927,7 +3117,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128">
       <c r="A128" t="s">
         <v>90</v>
       </c>
@@ -2938,7 +3128,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129">
       <c r="A129" t="s">
         <v>218</v>
       </c>
@@ -2949,7 +3139,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130">
       <c r="A130" t="s">
         <v>218</v>
       </c>
@@ -2960,7 +3150,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131">
       <c r="A131" t="s">
         <v>218</v>
       </c>
@@ -2971,7 +3161,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132">
       <c r="A132" t="s">
         <v>218</v>
       </c>
@@ -2982,7 +3172,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133">
       <c r="A133" t="s">
         <v>218</v>
       </c>
@@ -2993,7 +3183,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134">
       <c r="A134" t="s">
         <v>218</v>
       </c>
@@ -3004,7 +3194,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135">
       <c r="A135" t="s">
         <v>218</v>
       </c>
@@ -3015,7 +3205,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136">
       <c r="A136" t="s">
         <v>218</v>
       </c>
@@ -3026,7 +3216,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137">
       <c r="A137" t="s">
         <v>218</v>
       </c>
@@ -3037,7 +3227,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138">
       <c r="A138" t="s">
         <v>218</v>
       </c>
@@ -3048,7 +3238,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139">
       <c r="A139" t="s">
         <v>218</v>
       </c>
@@ -3059,7 +3249,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140">
       <c r="A140" t="s">
         <v>218</v>
       </c>
@@ -3070,7 +3260,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141">
       <c r="A141" t="s">
         <v>218</v>
       </c>
@@ -3081,7 +3271,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142">
       <c r="A142" t="s">
         <v>218</v>
       </c>
@@ -3092,7 +3282,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143">
       <c r="A143" t="s">
         <v>218</v>
       </c>
@@ -3103,7 +3293,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144">
       <c r="A144" t="s">
         <v>218</v>
       </c>
@@ -3114,7 +3304,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145">
       <c r="A145" t="s">
         <v>218</v>
       </c>
@@ -3125,7 +3315,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146">
       <c r="A146" t="s">
         <v>218</v>
       </c>
@@ -3136,7 +3326,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147">
       <c r="A147" t="s">
         <v>218</v>
       </c>
@@ -3147,7 +3337,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148">
       <c r="A148" t="s">
         <v>218</v>
       </c>
@@ -3158,7 +3348,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149">
       <c r="A149" t="s">
         <v>218</v>
       </c>
@@ -3169,7 +3359,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150">
       <c r="A150" t="s">
         <v>218</v>
       </c>
@@ -3180,7 +3370,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151">
       <c r="A151" t="s">
         <v>218</v>
       </c>
@@ -3191,7 +3381,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152">
       <c r="A152" t="s">
         <v>218</v>
       </c>
@@ -3202,7 +3392,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153">
       <c r="A153" t="s">
         <v>218</v>
       </c>
@@ -3213,7 +3403,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154">
       <c r="A154" t="s">
         <v>218</v>
       </c>
@@ -3224,7 +3414,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155">
       <c r="A155" t="s">
         <v>218</v>
       </c>
@@ -3235,7 +3425,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156">
       <c r="A156" t="s">
         <v>218</v>
       </c>
@@ -3246,7 +3436,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157">
       <c r="A157" t="s">
         <v>218</v>
       </c>
@@ -3257,7 +3447,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158">
       <c r="A158" t="s">
         <v>218</v>
       </c>
@@ -3268,7 +3458,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159">
       <c r="A159" t="s">
         <v>218</v>
       </c>
@@ -3279,7 +3469,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160">
       <c r="A160" t="s">
         <v>218</v>
       </c>
@@ -3290,7 +3480,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161">
       <c r="A161" t="s">
         <v>218</v>
       </c>
@@ -3301,7 +3491,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162">
       <c r="A162" t="s">
         <v>218</v>
       </c>
@@ -3312,7 +3502,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163">
       <c r="A163" t="s">
         <v>218</v>
       </c>
@@ -3323,7 +3513,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164">
       <c r="A164" t="s">
         <v>218</v>
       </c>
@@ -3334,7 +3524,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165">
       <c r="A165" t="s">
         <v>218</v>
       </c>
@@ -3345,7 +3535,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166">
       <c r="A166" t="s">
         <v>218</v>
       </c>
@@ -3356,7 +3546,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167">
       <c r="A167" t="s">
         <v>218</v>
       </c>
@@ -3367,7 +3557,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168">
       <c r="A168" t="s">
         <v>218</v>
       </c>
@@ -3378,7 +3568,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169">
       <c r="A169" t="s">
         <v>218</v>
       </c>
@@ -3389,7 +3579,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170">
       <c r="A170" t="s">
         <v>218</v>
       </c>
@@ -3400,7 +3590,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171">
       <c r="A171" t="s">
         <v>218</v>
       </c>
@@ -3411,7 +3601,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172">
       <c r="A172" t="s">
         <v>218</v>
       </c>
@@ -3422,7 +3612,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173">
       <c r="A173" t="s">
         <v>218</v>
       </c>
@@ -3433,7 +3623,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174">
       <c r="A174" t="s">
         <v>218</v>
       </c>
@@ -3444,7 +3634,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175">
       <c r="A175" t="s">
         <v>218</v>
       </c>
@@ -3455,7 +3645,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176">
       <c r="A176" t="s">
         <v>218</v>
       </c>
@@ -3466,7 +3656,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177">
       <c r="A177" t="s">
         <v>218</v>
       </c>
@@ -3477,7 +3667,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178">
       <c r="A178" t="s">
         <v>218</v>
       </c>
@@ -3488,7 +3678,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179">
       <c r="A179" t="s">
         <v>218</v>
       </c>
@@ -3499,7 +3689,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180">
       <c r="A180" t="s">
         <v>218</v>
       </c>
@@ -3510,7 +3700,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181">
       <c r="A181" t="s">
         <v>218</v>
       </c>
@@ -3521,7 +3711,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182">
       <c r="A182" t="s">
         <v>218</v>
       </c>
@@ -3532,7 +3722,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183">
       <c r="A183" t="s">
         <v>218</v>
       </c>
@@ -3543,7 +3733,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184">
       <c r="A184" t="s">
         <v>218</v>
       </c>
@@ -3554,7 +3744,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185">
       <c r="A185" t="s">
         <v>218</v>
       </c>
@@ -3565,7 +3755,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186">
       <c r="A186" t="s">
         <v>218</v>
       </c>
@@ -3576,7 +3766,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187">
       <c r="A187" t="s">
         <v>218</v>
       </c>
@@ -3587,7 +3777,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188">
       <c r="A188" t="s">
         <v>218</v>
       </c>
@@ -3598,7 +3788,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189">
       <c r="A189" t="s">
         <v>218</v>
       </c>
@@ -3609,7 +3799,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190">
       <c r="A190" t="s">
         <v>218</v>
       </c>
@@ -3620,7 +3810,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191">
       <c r="A191" t="s">
         <v>218</v>
       </c>
@@ -3631,7 +3821,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192">
       <c r="A192" t="s">
         <v>218</v>
       </c>
@@ -3642,7 +3832,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193">
       <c r="A193" t="s">
         <v>218</v>
       </c>
@@ -3653,7 +3843,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194">
       <c r="A194" t="s">
         <v>218</v>
       </c>
@@ -3664,7 +3854,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195">
       <c r="A195" t="s">
         <v>218</v>
       </c>
@@ -3675,7 +3865,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196">
       <c r="A196" t="s">
         <v>218</v>
       </c>
@@ -3686,7 +3876,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197">
       <c r="A197" t="s">
         <v>218</v>
       </c>
@@ -3697,7 +3887,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198">
       <c r="A198" t="s">
         <v>218</v>
       </c>
@@ -3708,7 +3898,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199">
       <c r="A199" t="s">
         <v>218</v>
       </c>
@@ -3719,7 +3909,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200">
       <c r="A200" t="s">
         <v>218</v>
       </c>
@@ -3730,7 +3920,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201">
       <c r="A201" t="s">
         <v>218</v>
       </c>
@@ -3741,7 +3931,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202">
       <c r="A202" t="s">
         <v>218</v>
       </c>
@@ -3752,7 +3942,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203">
       <c r="A203" t="s">
         <v>218</v>
       </c>
@@ -3763,7 +3953,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204">
       <c r="A204" t="s">
         <v>218</v>
       </c>
@@ -3774,7 +3964,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205">
       <c r="A205" t="s">
         <v>218</v>
       </c>
@@ -3785,7 +3975,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206">
       <c r="A206" t="s">
         <v>218</v>
       </c>
@@ -3796,7 +3986,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207">
       <c r="A207" t="s">
         <v>218</v>
       </c>
@@ -3807,7 +3997,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208">
       <c r="A208" t="s">
         <v>218</v>
       </c>
@@ -3818,7 +4008,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209">
       <c r="A209" t="s">
         <v>218</v>
       </c>
@@ -3829,7 +4019,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210">
       <c r="A210" t="s">
         <v>218</v>
       </c>
@@ -3840,7 +4030,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -3851,7 +4041,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -3862,7 +4052,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213">
       <c r="A213" t="s">
         <v>218</v>
       </c>
@@ -3873,7 +4063,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214">
       <c r="A214" t="s">
         <v>218</v>
       </c>
@@ -3884,7 +4074,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215">
       <c r="A215" t="s">
         <v>218</v>
       </c>
@@ -3895,7 +4085,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216">
       <c r="A216" t="s">
         <v>218</v>
       </c>
@@ -3906,7 +4096,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217">
       <c r="A217" t="s">
         <v>264</v>
       </c>
@@ -3917,7 +4107,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218">
       <c r="A218" t="s">
         <v>264</v>
       </c>
@@ -3928,7 +4118,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219">
       <c r="A219" t="s">
         <v>264</v>
       </c>
@@ -3939,7 +4129,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220">
       <c r="A220" t="s">
         <v>264</v>
       </c>
@@ -3950,7 +4140,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221">
       <c r="A221" t="s">
         <v>264</v>
       </c>
@@ -3961,7 +4151,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222">
       <c r="A222" t="s">
         <v>264</v>
       </c>
@@ -3972,7 +4162,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223">
       <c r="A223" t="s">
         <v>264</v>
       </c>
@@ -3983,7 +4173,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224">
       <c r="A224" t="s">
         <v>264</v>
       </c>
@@ -3994,7 +4184,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225">
       <c r="A225" t="s">
         <v>264</v>
       </c>
@@ -4005,7 +4195,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226">
       <c r="A226" t="s">
         <v>264</v>
       </c>
@@ -4016,7 +4206,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227">
       <c r="A227" t="s">
         <v>264</v>
       </c>
@@ -4027,7 +4217,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228">
       <c r="A228" t="s">
         <v>264</v>
       </c>
@@ -4038,7 +4228,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229">
       <c r="A229" t="s">
         <v>264</v>
       </c>
@@ -4049,7 +4239,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230">
       <c r="A230" t="s">
         <v>264</v>
       </c>
@@ -4060,7 +4250,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231">
       <c r="A231" t="s">
         <v>264</v>
       </c>
@@ -4071,7 +4261,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232">
       <c r="A232" t="s">
         <v>264</v>
       </c>
@@ -4082,7 +4272,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233">
       <c r="A233" t="s">
         <v>264</v>
       </c>
@@ -4093,7 +4283,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234">
       <c r="A234" t="s">
         <v>264</v>
       </c>
@@ -4104,7 +4294,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235">
       <c r="A235" t="s">
         <v>264</v>
       </c>
@@ -4115,7 +4305,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236">
       <c r="A236" t="s">
         <v>264</v>
       </c>
@@ -4126,7 +4316,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237">
       <c r="A237" t="s">
         <v>264</v>
       </c>
@@ -4137,7 +4327,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238">
       <c r="A238" t="s">
         <v>264</v>
       </c>
@@ -4148,7 +4338,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239">
       <c r="A239" t="s">
         <v>291</v>
       </c>
@@ -4159,7 +4349,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240">
       <c r="A240" t="s">
         <v>291</v>
       </c>
@@ -4170,7 +4360,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241">
       <c r="A241" t="s">
         <v>291</v>
       </c>
@@ -4181,7 +4371,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242">
       <c r="A242" t="s">
         <v>291</v>
       </c>
@@ -4192,7 +4382,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243">
       <c r="A243" t="s">
         <v>291</v>
       </c>
@@ -4203,7 +4393,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244">
       <c r="A244" t="s">
         <v>291</v>
       </c>
@@ -4214,7 +4404,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245">
       <c r="A245" t="s">
         <v>291</v>
       </c>
@@ -4225,7 +4415,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246">
       <c r="A246" t="s">
         <v>291</v>
       </c>
@@ -4236,7 +4426,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247">
       <c r="A247" t="s">
         <v>291</v>
       </c>
@@ -4247,7 +4437,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248">
       <c r="A248" t="s">
         <v>291</v>
       </c>
@@ -4258,7 +4448,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249">
       <c r="A249" t="s">
         <v>291</v>
       </c>
@@ -4269,7 +4459,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250">
       <c r="A250" t="s">
         <v>291</v>
       </c>
@@ -4280,7 +4470,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251">
       <c r="A251" t="s">
         <v>291</v>
       </c>
@@ -4291,7 +4481,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252">
       <c r="A252" t="s">
         <v>291</v>
       </c>
@@ -4302,7 +4492,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253">
       <c r="A253" t="s">
         <v>291</v>
       </c>
@@ -4313,7 +4503,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254">
       <c r="A254" t="s">
         <v>291</v>
       </c>
@@ -4324,7 +4514,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255">
       <c r="A255" t="s">
         <v>291</v>
       </c>
@@ -4335,7 +4525,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256">
       <c r="A256" t="s">
         <v>291</v>
       </c>
@@ -4346,7 +4536,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257">
       <c r="A257" t="s">
         <v>291</v>
       </c>
@@ -4357,7 +4547,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258">
       <c r="A258" t="s">
         <v>291</v>
       </c>
@@ -4368,7 +4558,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="259">
       <c r="A259" t="s">
         <v>291</v>
       </c>
@@ -4379,7 +4569,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260">
       <c r="A260" t="s">
         <v>291</v>
       </c>
@@ -4394,4 +4584,375 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>346</v>
+      </c>
+      <c r="B7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="s">
+        <v>351</v>
+      </c>
+      <c r="C9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" t="s">
+        <v>353</v>
+      </c>
+      <c r="C10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>356</v>
+      </c>
+      <c r="B12" t="s">
+        <v>357</v>
+      </c>
+      <c r="C12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>360</v>
+      </c>
+      <c r="B14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B15" t="s">
+        <v>363</v>
+      </c>
+      <c r="C15" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>364</v>
+      </c>
+      <c r="B16" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>366</v>
+      </c>
+      <c r="B17" t="s">
+        <v>367</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>369</v>
+      </c>
+      <c r="B19" t="s">
+        <v>370</v>
+      </c>
+      <c r="C19" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>371</v>
+      </c>
+      <c r="B20"/>
+      <c r="C20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>372</v>
+      </c>
+      <c r="B21" t="s">
+        <v>367</v>
+      </c>
+      <c r="C21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>373</v>
+      </c>
+      <c r="B22" t="s">
+        <v>374</v>
+      </c>
+      <c r="C22" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B23" t="s">
+        <v>376</v>
+      </c>
+      <c r="C23" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>377</v>
+      </c>
+      <c r="B24" t="s">
+        <v>378</v>
+      </c>
+      <c r="C24" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>379</v>
+      </c>
+      <c r="B25" t="s">
+        <v>380</v>
+      </c>
+      <c r="C25" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>381</v>
+      </c>
+      <c r="B26" t="s">
+        <v>382</v>
+      </c>
+      <c r="C26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>383</v>
+      </c>
+      <c r="B27" t="s">
+        <v>376</v>
+      </c>
+      <c r="C27" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>384</v>
+      </c>
+      <c r="B28" t="s">
+        <v>378</v>
+      </c>
+      <c r="C28" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>385</v>
+      </c>
+      <c r="B29" t="s">
+        <v>386</v>
+      </c>
+      <c r="C29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>387</v>
+      </c>
+      <c r="B30" t="s">
+        <v>388</v>
+      </c>
+      <c r="C30" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B31" t="s">
+        <v>390</v>
+      </c>
+      <c r="C31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>392</v>
+      </c>
+      <c r="B32"/>
+      <c r="C32" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>393</v>
+      </c>
+      <c r="B33" t="s">
+        <v>394</v>
+      </c>
+      <c r="C33" t="s">
+        <v>391</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>